<commit_message>
Named sub menu buttons
</commit_message>
<xml_diff>
--- a/product_backlog.xlsx
+++ b/product_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <t>Priority (1 - Most Urgent, 5 - Least)</t>
   </si>
   <si>
-    <t>first objective</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -476,23 +476,23 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -507,7 +507,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -520,7 +520,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -552,7 +552,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -586,9 +586,9 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -603,7 +603,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -616,7 +616,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -629,7 +629,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -642,7 +642,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -655,7 +655,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -668,7 +668,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -681,7 +681,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -694,7 +694,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -707,7 +707,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -720,7 +720,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -733,7 +733,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -746,7 +746,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -759,7 +759,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -772,7 +772,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -785,7 +785,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -798,7 +798,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -811,7 +811,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -839,7 +839,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -851,7 +851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>